<commit_message>
"permission added and api duplicate object fixed"
</commit_message>
<xml_diff>
--- a/TrainingLogFormat.xlsx
+++ b/TrainingLogFormat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="17175" windowHeight="10755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="17175" windowHeight="10755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Client Details" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -828,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
"Workout Creation API - Added (Excel Parse)"
</commit_message>
<xml_diff>
--- a/TrainingLogFormat.xlsx
+++ b/TrainingLogFormat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="17175" windowHeight="10755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="17175" windowHeight="10755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Client Details" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="56">
   <si>
     <t>Day</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Leg Press</t>
+  </si>
+  <si>
+    <t>parallel to ground</t>
+  </si>
+  <si>
+    <t>pause at lowest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slow negatives </t>
   </si>
 </sst>
 </file>
@@ -568,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -646,7 +655,7 @@
         <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -798,6 +807,15 @@
       <c r="G11" t="s">
         <v>51</v>
       </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="E12" t="s">
@@ -805,6 +823,15 @@
       </c>
       <c r="G12" t="s">
         <v>52</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>